<commit_message>
fix calculations on tech tree calculator
</commit_message>
<xml_diff>
--- a/stats editor/tech_tree_test/results.xlsx
+++ b/stats editor/tech_tree_test/results.xlsx
@@ -1600,7 +1600,7 @@
         <v>1200</v>
       </c>
       <c r="E2">
-        <v>85.71428571428571</v>
+        <v>171.4285714285714</v>
       </c>
       <c r="F2">
         <v>32.43243243243244</v>
@@ -1620,7 +1620,7 @@
         <v>900</v>
       </c>
       <c r="E3">
-        <v>64.28571428571429</v>
+        <v>128.5714285714286</v>
       </c>
       <c r="F3">
         <v>32.14285714285715</v>
@@ -1640,7 +1640,7 @@
         <v>60</v>
       </c>
       <c r="E4">
-        <v>4.285714285714286</v>
+        <v>8.571428571428571</v>
       </c>
       <c r="F4">
         <v>60</v>
@@ -1660,7 +1660,7 @@
         <v>1200</v>
       </c>
       <c r="E5">
-        <v>85.71428571428571</v>
+        <v>171.4285714285714</v>
       </c>
       <c r="F5">
         <v>32.43243243243244</v>
@@ -1680,7 +1680,7 @@
         <v>1200</v>
       </c>
       <c r="E6">
-        <v>85.71428571428571</v>
+        <v>171.4285714285714</v>
       </c>
       <c r="F6">
         <v>32.43243243243244</v>
@@ -1700,7 +1700,7 @@
         <v>600</v>
       </c>
       <c r="E7">
-        <v>42.85714285714285</v>
+        <v>85.71428571428571</v>
       </c>
       <c r="F7">
         <v>33.33333333333334</v>
@@ -1720,7 +1720,7 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>0.7142857142857143</v>
+        <v>1.428571428571429</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1740,7 +1740,7 @@
         <v>600</v>
       </c>
       <c r="E9">
-        <v>128.5714285714286</v>
+        <v>171.4285714285714</v>
       </c>
       <c r="F9">
         <v>33.33333333333334</v>
@@ -1760,7 +1760,7 @@
         <v>600</v>
       </c>
       <c r="E10">
-        <v>128.5714285714286</v>
+        <v>171.4285714285714</v>
       </c>
       <c r="F10">
         <v>33.33333333333334</v>
@@ -1780,7 +1780,7 @@
         <v>600</v>
       </c>
       <c r="E11">
-        <v>47.14285714285715</v>
+        <v>90</v>
       </c>
       <c r="F11">
         <v>33.33333333333334</v>
@@ -1800,7 +1800,7 @@
         <v>1800</v>
       </c>
       <c r="E12">
-        <v>214.2857142857143</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F12">
         <v>32.14285714285715</v>
@@ -1820,7 +1820,7 @@
         <v>1200</v>
       </c>
       <c r="E13">
-        <v>171.4285714285714</v>
+        <v>257.1428571428571</v>
       </c>
       <c r="F13">
         <v>32.43243243243244</v>
@@ -1840,7 +1840,7 @@
         <v>600</v>
       </c>
       <c r="E14">
-        <v>128.5714285714286</v>
+        <v>171.4285714285714</v>
       </c>
       <c r="F14">
         <v>33.33333333333334</v>
@@ -1860,7 +1860,7 @@
         <v>900</v>
       </c>
       <c r="E15">
-        <v>128.5714285714286</v>
+        <v>192.8571428571429</v>
       </c>
       <c r="F15">
         <v>32.14285714285715</v>
@@ -1880,7 +1880,7 @@
         <v>2400</v>
       </c>
       <c r="E16">
-        <v>257.1428571428572</v>
+        <v>428.5714285714286</v>
       </c>
       <c r="F16">
         <v>32</v>
@@ -1900,7 +1900,7 @@
         <v>1200</v>
       </c>
       <c r="E17">
-        <v>171.4285714285714</v>
+        <v>257.1428571428571</v>
       </c>
       <c r="F17">
         <v>32.43243243243244</v>
@@ -1920,7 +1920,7 @@
         <v>600</v>
       </c>
       <c r="E18">
-        <v>128.5714285714286</v>
+        <v>171.4285714285714</v>
       </c>
       <c r="F18">
         <v>33.33333333333334</v>
@@ -1940,7 +1940,7 @@
         <v>600</v>
       </c>
       <c r="E19">
-        <v>47.14285714285715</v>
+        <v>90</v>
       </c>
       <c r="F19">
         <v>33.33333333333334</v>
@@ -1960,7 +1960,7 @@
         <v>1200</v>
       </c>
       <c r="E20">
-        <v>171.4285714285714</v>
+        <v>257.1428571428571</v>
       </c>
       <c r="F20">
         <v>32.43243243243244</v>
@@ -1980,7 +1980,7 @@
         <v>1800</v>
       </c>
       <c r="E21">
-        <v>257.1428571428572</v>
+        <v>385.7142857142858</v>
       </c>
       <c r="F21">
         <v>32.14285714285715</v>
@@ -2000,7 +2000,7 @@
         <v>1200</v>
       </c>
       <c r="E22">
-        <v>132.8571428571429</v>
+        <v>218.5714285714286</v>
       </c>
       <c r="F22">
         <v>32.43243243243244</v>
@@ -2020,7 +2020,7 @@
         <v>1500</v>
       </c>
       <c r="E23">
-        <v>235.7142857142857</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F23">
         <v>32.60869565217391</v>
@@ -2040,7 +2040,7 @@
         <v>2400</v>
       </c>
       <c r="E24">
-        <v>235.7142857142857</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F24">
         <v>32</v>
@@ -2060,7 +2060,7 @@
         <v>1200</v>
       </c>
       <c r="E25">
-        <v>214.2857142857143</v>
+        <v>300</v>
       </c>
       <c r="F25">
         <v>32.43243243243244</v>
@@ -2080,7 +2080,7 @@
         <v>1200</v>
       </c>
       <c r="E26">
-        <v>214.2857142857143</v>
+        <v>300</v>
       </c>
       <c r="F26">
         <v>32.43243243243244</v>
@@ -2100,7 +2100,7 @@
         <v>2400</v>
       </c>
       <c r="E27">
-        <v>328.5714285714286</v>
+        <v>442.8571428571428</v>
       </c>
       <c r="F27">
         <v>32</v>
@@ -2120,7 +2120,7 @@
         <v>1200</v>
       </c>
       <c r="E28">
-        <v>214.2857142857143</v>
+        <v>300</v>
       </c>
       <c r="F28">
         <v>32.43243243243244</v>
@@ -2140,7 +2140,7 @@
         <v>4800</v>
       </c>
       <c r="E29">
-        <v>1505.951556380128</v>
+        <v>1601.189651618223</v>
       </c>
       <c r="F29">
         <v>32</v>
@@ -2160,7 +2160,7 @@
         <v>1800</v>
       </c>
       <c r="E30">
-        <v>175.7142857142857</v>
+        <v>304.2857142857143</v>
       </c>
       <c r="F30">
         <v>32.14285714285715</v>
@@ -2180,7 +2180,7 @@
         <v>600</v>
       </c>
       <c r="E31">
-        <v>171.4285714285714</v>
+        <v>214.2857142857143</v>
       </c>
       <c r="F31">
         <v>33.33333333333334</v>
@@ -2200,7 +2200,7 @@
         <v>1200</v>
       </c>
       <c r="E32">
-        <v>132.8571428571429</v>
+        <v>218.5714285714286</v>
       </c>
       <c r="F32">
         <v>32.43243243243244</v>
@@ -2220,7 +2220,7 @@
         <v>1200</v>
       </c>
       <c r="E33">
-        <v>257.1428571428572</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F33">
         <v>32.43243243243244</v>
@@ -2240,7 +2240,7 @@
         <v>1200</v>
       </c>
       <c r="E34">
-        <v>257.1428571428572</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F34">
         <v>32.43243243243244</v>
@@ -2260,7 +2260,7 @@
         <v>1500</v>
       </c>
       <c r="E35">
-        <v>235.7142857142857</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F35">
         <v>32.60869565217391</v>
@@ -2280,7 +2280,7 @@
         <v>1500</v>
       </c>
       <c r="E36">
-        <v>235.7142857142857</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F36">
         <v>32.60869565217391</v>
@@ -2300,7 +2300,7 @@
         <v>2400</v>
       </c>
       <c r="E37">
-        <v>235.7142857142857</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F37">
         <v>32</v>
@@ -2320,7 +2320,7 @@
         <v>2400</v>
       </c>
       <c r="E38">
-        <v>1482.142032570604</v>
+        <v>1529.761080189652</v>
       </c>
       <c r="F38">
         <v>32</v>
@@ -2340,7 +2340,7 @@
         <v>1200</v>
       </c>
       <c r="E39">
-        <v>1482.142032570604</v>
+        <v>1529.761080189652</v>
       </c>
       <c r="F39">
         <v>32.43243243243244</v>
@@ -2360,7 +2360,7 @@
         <v>2400</v>
       </c>
       <c r="E40">
-        <v>1482.142032570604</v>
+        <v>1529.761080189652</v>
       </c>
       <c r="F40">
         <v>32</v>
@@ -2380,7 +2380,7 @@
         <v>1200</v>
       </c>
       <c r="E41">
-        <v>1482.142032570604</v>
+        <v>1529.761080189652</v>
       </c>
       <c r="F41">
         <v>32.43243243243244</v>
@@ -2400,7 +2400,7 @@
         <v>1200</v>
       </c>
       <c r="E42">
-        <v>1458.33250876108</v>
+        <v>1482.142032570604</v>
       </c>
       <c r="F42">
         <v>32.43243243243244</v>
@@ -2420,7 +2420,7 @@
         <v>3600</v>
       </c>
       <c r="E43">
-        <v>1482.142032570604</v>
+        <v>1553.570603999175</v>
       </c>
       <c r="F43">
         <v>32.14285714285715</v>
@@ -2440,7 +2440,7 @@
         <v>1200</v>
       </c>
       <c r="E44">
-        <v>261.4285714285714</v>
+        <v>347.1428571428572</v>
       </c>
       <c r="F44">
         <v>32.43243243243244</v>
@@ -2460,7 +2460,7 @@
         <v>1200</v>
       </c>
       <c r="E45">
-        <v>257.1428571428572</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F45">
         <v>32.43243243243244</v>
@@ -2480,7 +2480,7 @@
         <v>1200</v>
       </c>
       <c r="E46">
-        <v>218.5714285714286</v>
+        <v>304.2857142857143</v>
       </c>
       <c r="F46">
         <v>32.43243243243244</v>
@@ -2500,7 +2500,7 @@
         <v>2400</v>
       </c>
       <c r="E47">
-        <v>1458.33250876108</v>
+        <v>1505.951556380128</v>
       </c>
       <c r="F47">
         <v>32</v>
@@ -2520,7 +2520,7 @@
         <v>1200</v>
       </c>
       <c r="E48">
-        <v>1458.33250876108</v>
+        <v>1505.951556380128</v>
       </c>
       <c r="F48">
         <v>32.43243243243244</v>
@@ -2540,7 +2540,7 @@
         <v>3600</v>
       </c>
       <c r="E49">
-        <v>1517.85631828489</v>
+        <v>1589.284889713461</v>
       </c>
       <c r="F49">
         <v>32.14285714285715</v>
@@ -2560,7 +2560,7 @@
         <v>2400</v>
       </c>
       <c r="E50">
-        <v>1470.237270665842</v>
+        <v>1517.85631828489</v>
       </c>
       <c r="F50">
         <v>32</v>
@@ -2580,7 +2580,7 @@
         <v>1200</v>
       </c>
       <c r="E51">
-        <v>1470.237270665842</v>
+        <v>1517.85631828489</v>
       </c>
       <c r="F51">
         <v>32.43243243243244</v>
@@ -2600,7 +2600,7 @@
         <v>2400</v>
       </c>
       <c r="E52">
-        <v>1470.237270665842</v>
+        <v>1517.85631828489</v>
       </c>
       <c r="F52">
         <v>32</v>
@@ -2620,7 +2620,7 @@
         <v>1800</v>
       </c>
       <c r="E53">
-        <v>1458.33250876108</v>
+        <v>1494.046794475366</v>
       </c>
       <c r="F53">
         <v>32.14285714285715</v>
@@ -2640,7 +2640,7 @@
         <v>6000</v>
       </c>
       <c r="E54">
-        <v>1601.189651618223</v>
+        <v>1720.237270665842</v>
       </c>
       <c r="F54">
         <v>32.0855614973262</v>
@@ -2660,7 +2660,7 @@
         <v>3600</v>
       </c>
       <c r="E55">
-        <v>1471.427746856318</v>
+        <v>1542.85631828489</v>
       </c>
       <c r="F55">
         <v>32.14285714285715</v>
@@ -2680,7 +2680,7 @@
         <v>2400</v>
       </c>
       <c r="E56">
-        <v>1459.522984951556</v>
+        <v>1507.142032570604</v>
       </c>
       <c r="F56">
         <v>32</v>
@@ -2700,7 +2700,7 @@
         <v>3600</v>
       </c>
       <c r="E57">
-        <v>1483.33250876108</v>
+        <v>1554.761080189651</v>
       </c>
       <c r="F57">
         <v>32.14285714285715</v>
@@ -2720,7 +2720,7 @@
         <v>2400</v>
       </c>
       <c r="E58">
-        <v>1458.33250876108</v>
+        <v>1505.951556380128</v>
       </c>
       <c r="F58">
         <v>32</v>
@@ -2740,7 +2740,7 @@
         <v>900</v>
       </c>
       <c r="E59">
-        <v>314.2857142857143</v>
+        <v>357.1428571428571</v>
       </c>
       <c r="F59">
         <v>32.14285714285715</v>
@@ -2760,7 +2760,7 @@
         <v>2400</v>
       </c>
       <c r="E60">
-        <v>302.8571428571428</v>
+        <v>417.1428571428571</v>
       </c>
       <c r="F60">
         <v>32</v>
@@ -2780,7 +2780,7 @@
         <v>2400</v>
       </c>
       <c r="E61">
-        <v>1459.522984951556</v>
+        <v>1507.142032570604</v>
       </c>
       <c r="F61">
         <v>32</v>
@@ -2800,7 +2800,7 @@
         <v>3600</v>
       </c>
       <c r="E62">
-        <v>1529.761080189652</v>
+        <v>1601.189651618223</v>
       </c>
       <c r="F62">
         <v>32.14285714285715</v>
@@ -2820,7 +2820,7 @@
         <v>2400</v>
       </c>
       <c r="E63">
-        <v>1505.951556380128</v>
+        <v>1553.570603999176</v>
       </c>
       <c r="F63">
         <v>32</v>
@@ -2840,7 +2840,7 @@
         <v>2400</v>
       </c>
       <c r="E64">
-        <v>1505.951556380128</v>
+        <v>1553.570603999176</v>
       </c>
       <c r="F64">
         <v>32</v>
@@ -2860,7 +2860,7 @@
         <v>2400</v>
       </c>
       <c r="E65">
-        <v>1505.951556380128</v>
+        <v>1553.570603999176</v>
       </c>
       <c r="F65">
         <v>32</v>
@@ -2880,7 +2880,7 @@
         <v>3600</v>
       </c>
       <c r="E66">
-        <v>1542.85631828489</v>
+        <v>1614.284889713461</v>
       </c>
       <c r="F66">
         <v>32.14285714285715</v>
@@ -2900,7 +2900,7 @@
         <v>1200</v>
       </c>
       <c r="E67">
-        <v>214.2857142857143</v>
+        <v>300</v>
       </c>
       <c r="F67">
         <v>32.43243243243244</v>
@@ -2920,7 +2920,7 @@
         <v>1200</v>
       </c>
       <c r="E68">
-        <v>214.2857142857143</v>
+        <v>300</v>
       </c>
       <c r="F68">
         <v>32.43243243243244</v>
@@ -2940,7 +2940,7 @@
         <v>1800</v>
       </c>
       <c r="E69">
-        <v>342.8571428571428</v>
+        <v>428.5714285714286</v>
       </c>
       <c r="F69">
         <v>32.14285714285715</v>
@@ -2960,7 +2960,7 @@
         <v>3600</v>
       </c>
       <c r="E70">
-        <v>1541.665842094414</v>
+        <v>1613.094413522985</v>
       </c>
       <c r="F70">
         <v>32.14285714285715</v>
@@ -2980,7 +2980,7 @@
         <v>2400</v>
       </c>
       <c r="E71">
-        <v>1541.665842094414</v>
+        <v>1613.094413522985</v>
       </c>
       <c r="F71">
         <v>32</v>
@@ -3000,7 +3000,7 @@
         <v>6000</v>
       </c>
       <c r="E72">
-        <v>1720.237270665842</v>
+        <v>1839.284889713461</v>
       </c>
       <c r="F72">
         <v>32.0855614973262</v>
@@ -3020,7 +3020,7 @@
         <v>1200</v>
       </c>
       <c r="E73">
-        <v>1482.142032570604</v>
+        <v>1505.951556380128</v>
       </c>
       <c r="F73">
         <v>32.43243243243244</v>
@@ -3040,7 +3040,7 @@
         <v>3600</v>
       </c>
       <c r="E74">
-        <v>1529.761080189652</v>
+        <v>1601.189651618223</v>
       </c>
       <c r="F74">
         <v>32.14285714285715</v>
@@ -3060,7 +3060,7 @@
         <v>6000</v>
       </c>
       <c r="E75">
-        <v>1590.475365903937</v>
+        <v>1709.522984951556</v>
       </c>
       <c r="F75">
         <v>32.0855614973262</v>
@@ -3080,7 +3080,7 @@
         <v>5500</v>
       </c>
       <c r="E76">
-        <v>1710.316635745207</v>
+        <v>1819.443619872191</v>
       </c>
       <c r="F76">
         <v>32.16374269005848</v>
@@ -3100,7 +3100,7 @@
         <v>3600</v>
       </c>
       <c r="E77">
-        <v>1517.85631828489</v>
+        <v>1589.284889713461</v>
       </c>
       <c r="F77">
         <v>32.14285714285715</v>
@@ -3120,7 +3120,7 @@
         <v>3600</v>
       </c>
       <c r="E78">
-        <v>1530.951556380128</v>
+        <v>1602.380127808699</v>
       </c>
       <c r="F78">
         <v>32.14285714285715</v>
@@ -3140,7 +3140,7 @@
         <v>7200</v>
       </c>
       <c r="E79">
-        <v>1601.189651618223</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F79">
         <v>32</v>
@@ -3160,7 +3160,7 @@
         <v>7200</v>
       </c>
       <c r="E80">
-        <v>1566.665842094414</v>
+        <v>1709.522984951557</v>
       </c>
       <c r="F80">
         <v>32</v>
@@ -3180,7 +3180,7 @@
         <v>3600</v>
       </c>
       <c r="E81">
-        <v>1495.237270665842</v>
+        <v>1566.665842094413</v>
       </c>
       <c r="F81">
         <v>32.14285714285715</v>
@@ -3200,7 +3200,7 @@
         <v>2400</v>
       </c>
       <c r="E82">
-        <v>1447.618223046794</v>
+        <v>1495.237270665842</v>
       </c>
       <c r="F82">
         <v>32</v>
@@ -3220,7 +3220,7 @@
         <v>1800</v>
       </c>
       <c r="E83">
-        <v>1495.237270665842</v>
+        <v>1530.951556380128</v>
       </c>
       <c r="F83">
         <v>32.14285714285715</v>
@@ -3240,7 +3240,7 @@
         <v>3600</v>
       </c>
       <c r="E84">
-        <v>1517.85631828489</v>
+        <v>1589.284889713461</v>
       </c>
       <c r="F84">
         <v>32.14285714285715</v>
@@ -3260,7 +3260,7 @@
         <v>4800</v>
       </c>
       <c r="E85">
-        <v>1601.189651618223</v>
+        <v>1696.427746856318</v>
       </c>
       <c r="F85">
         <v>32</v>
@@ -3280,7 +3280,7 @@
         <v>3600</v>
       </c>
       <c r="E86">
-        <v>1601.189651618223</v>
+        <v>1696.427746856318</v>
       </c>
       <c r="F86">
         <v>32.14285714285715</v>
@@ -3300,7 +3300,7 @@
         <v>3600</v>
       </c>
       <c r="E87">
-        <v>1470.237270665842</v>
+        <v>1541.665842094413</v>
       </c>
       <c r="F87">
         <v>32.14285714285715</v>
@@ -3320,7 +3320,7 @@
         <v>1200</v>
       </c>
       <c r="E88">
-        <v>214.2857142857143</v>
+        <v>300</v>
       </c>
       <c r="F88">
         <v>32.43243243243244</v>
@@ -3340,7 +3340,7 @@
         <v>3600</v>
       </c>
       <c r="E89">
-        <v>214.2857142857143</v>
+        <v>300</v>
       </c>
       <c r="F89">
         <v>32.14285714285715</v>
@@ -3360,7 +3360,7 @@
         <v>3600</v>
       </c>
       <c r="E90">
-        <v>1672.618223046794</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F90">
         <v>32.14285714285715</v>
@@ -3380,7 +3380,7 @@
         <v>2400</v>
       </c>
       <c r="E91">
-        <v>1529.761080189652</v>
+        <v>1577.380127808699</v>
       </c>
       <c r="F91">
         <v>32</v>
@@ -3400,7 +3400,7 @@
         <v>2400</v>
       </c>
       <c r="E92">
-        <v>1505.951556380128</v>
+        <v>1553.570603999176</v>
       </c>
       <c r="F92">
         <v>32</v>
@@ -3420,7 +3420,7 @@
         <v>5400</v>
       </c>
       <c r="E93">
-        <v>1636.903937332509</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F93">
         <v>32.14285714285715</v>
@@ -3440,7 +3440,7 @@
         <v>2400</v>
       </c>
       <c r="E94">
-        <v>328.5714285714286</v>
+        <v>442.8571428571428</v>
       </c>
       <c r="F94">
         <v>32</v>
@@ -3460,7 +3460,7 @@
         <v>7200</v>
       </c>
       <c r="E95">
-        <v>1733.33250876108</v>
+        <v>1876.189651618223</v>
       </c>
       <c r="F95">
         <v>32</v>
@@ -3480,7 +3480,7 @@
         <v>3600</v>
       </c>
       <c r="E96">
-        <v>1566.665842094414</v>
+        <v>1638.094413522985</v>
       </c>
       <c r="F96">
         <v>32.14285714285715</v>
@@ -3500,7 +3500,7 @@
         <v>7200</v>
       </c>
       <c r="E97">
-        <v>1601.189651618223</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F97">
         <v>32</v>
@@ -3520,7 +3520,7 @@
         <v>6000</v>
       </c>
       <c r="E98">
-        <v>1649.999175427747</v>
+        <v>1769.046794475366</v>
       </c>
       <c r="F98">
         <v>32.0855614973262</v>
@@ -3540,7 +3540,7 @@
         <v>4800</v>
       </c>
       <c r="E99">
-        <v>1483.33250876108</v>
+        <v>1578.570603999175</v>
       </c>
       <c r="F99">
         <v>32</v>
@@ -3560,7 +3560,7 @@
         <v>7200</v>
       </c>
       <c r="E100">
-        <v>1517.85631828489</v>
+        <v>1660.713461142033</v>
       </c>
       <c r="F100">
         <v>32</v>
@@ -3580,7 +3580,7 @@
         <v>9200</v>
       </c>
       <c r="E101">
-        <v>1783.729334157905</v>
+        <v>1966.269016697588</v>
       </c>
       <c r="F101">
         <v>32.05574912891986</v>
@@ -3600,7 +3600,7 @@
         <v>9200</v>
       </c>
       <c r="E102">
-        <v>1677.776953205524</v>
+        <v>1860.316635745207</v>
       </c>
       <c r="F102">
         <v>32.05574912891986</v>
@@ -3620,7 +3620,7 @@
         <v>4800</v>
       </c>
       <c r="E103">
-        <v>1590.475365903937</v>
+        <v>1685.713461142032</v>
       </c>
       <c r="F103">
         <v>32</v>
@@ -3640,7 +3640,7 @@
         <v>3600</v>
       </c>
       <c r="E104">
-        <v>1590.475365903937</v>
+        <v>1685.713461142032</v>
       </c>
       <c r="F104">
         <v>32.14285714285715</v>
@@ -3660,7 +3660,7 @@
         <v>3600</v>
       </c>
       <c r="E105">
-        <v>1566.665842094414</v>
+        <v>1638.094413522985</v>
       </c>
       <c r="F105">
         <v>32.14285714285715</v>
@@ -3680,7 +3680,7 @@
         <v>9600</v>
       </c>
       <c r="E106">
-        <v>1791.665842094413</v>
+        <v>1982.142032570604</v>
       </c>
       <c r="F106">
         <v>32</v>
@@ -3700,7 +3700,7 @@
         <v>3600</v>
       </c>
       <c r="E107">
-        <v>1589.284889713461</v>
+        <v>1660.713461142032</v>
       </c>
       <c r="F107">
         <v>32.14285714285715</v>
@@ -3720,7 +3720,7 @@
         <v>3600</v>
       </c>
       <c r="E108">
-        <v>1636.903937332509</v>
+        <v>1708.33250876108</v>
       </c>
       <c r="F108">
         <v>32.14285714285715</v>
@@ -3740,7 +3740,7 @@
         <v>3200</v>
       </c>
       <c r="E109">
-        <v>1546.824572253144</v>
+        <v>1610.316635745207</v>
       </c>
       <c r="F109">
         <v>32</v>
@@ -3760,7 +3760,7 @@
         <v>4000</v>
       </c>
       <c r="E110">
-        <v>1597.221397649969</v>
+        <v>1676.586477015048</v>
       </c>
       <c r="F110">
         <v>32</v>
@@ -3780,7 +3780,7 @@
         <v>1500</v>
       </c>
       <c r="E111">
-        <v>235.7142857142857</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F111">
         <v>32.60869565217391</v>
@@ -3800,7 +3800,7 @@
         <v>4800</v>
       </c>
       <c r="E112">
-        <v>1578.570603999176</v>
+        <v>1673.808699237271</v>
       </c>
       <c r="F112">
         <v>32</v>
@@ -3820,7 +3820,7 @@
         <v>1500</v>
       </c>
       <c r="E113">
-        <v>235.7142857142857</v>
+        <v>342.8571428571429</v>
       </c>
       <c r="F113">
         <v>32.60869565217391</v>
@@ -3840,7 +3840,7 @@
         <v>9200</v>
       </c>
       <c r="E114">
-        <v>1664.681715110286</v>
+        <v>1847.221397649969</v>
       </c>
       <c r="F114">
         <v>32.05574912891986</v>
@@ -3860,7 +3860,7 @@
         <v>4800</v>
       </c>
       <c r="E115">
-        <v>1664.681715110286</v>
+        <v>1847.221397649969</v>
       </c>
       <c r="F115">
         <v>32</v>
@@ -3880,7 +3880,7 @@
         <v>4800</v>
       </c>
       <c r="E116">
-        <v>1767.85631828489</v>
+        <v>1863.094413522985</v>
       </c>
       <c r="F116">
         <v>32</v>
@@ -3900,7 +3900,7 @@
         <v>4000</v>
       </c>
       <c r="E117">
-        <v>1549.602350030922</v>
+        <v>1628.967429396001</v>
       </c>
       <c r="F117">
         <v>32</v>
@@ -3920,7 +3920,7 @@
         <v>4800</v>
       </c>
       <c r="E118">
-        <v>1732.142032570604</v>
+        <v>1827.380127808699</v>
       </c>
       <c r="F118">
         <v>32</v>
@@ -3940,7 +3940,7 @@
         <v>8400</v>
       </c>
       <c r="E119">
-        <v>1899.999175427747</v>
+        <v>2066.665842094413</v>
       </c>
       <c r="F119">
         <v>32.06106870229008</v>
@@ -3960,7 +3960,7 @@
         <v>4800</v>
       </c>
       <c r="E120">
-        <v>1661.903937332509</v>
+        <v>1757.142032570604</v>
       </c>
       <c r="F120">
         <v>32</v>
@@ -3980,7 +3980,7 @@
         <v>7200</v>
       </c>
       <c r="E121">
-        <v>1626.189651618223</v>
+        <v>1769.046794475366</v>
       </c>
       <c r="F121">
         <v>32</v>
@@ -4000,7 +4000,7 @@
         <v>9200</v>
       </c>
       <c r="E122">
-        <v>1783.729334157905</v>
+        <v>1966.269016697588</v>
       </c>
       <c r="F122">
         <v>32.05574912891986</v>
@@ -4020,7 +4020,7 @@
         <v>7200</v>
       </c>
       <c r="E123">
-        <v>1792.85631828489</v>
+        <v>1935.713461142032</v>
       </c>
       <c r="F123">
         <v>32</v>
@@ -4040,7 +4040,7 @@
         <v>4000</v>
       </c>
       <c r="E124">
-        <v>1729.364254792826</v>
+        <v>1808.729334157905</v>
       </c>
       <c r="F124">
         <v>32</v>
@@ -4060,7 +4060,7 @@
         <v>11200</v>
       </c>
       <c r="E125">
-        <v>2005.951556380128</v>
+        <v>2228.17377860235</v>
       </c>
       <c r="F125">
         <v>32</v>
@@ -4080,7 +4080,7 @@
         <v>6000</v>
       </c>
       <c r="E126">
-        <v>1547.618223046794</v>
+        <v>1666.665842094413</v>
       </c>
       <c r="F126">
         <v>32.0855614973262</v>
@@ -4100,7 +4100,7 @@
         <v>11200</v>
       </c>
       <c r="E127">
-        <v>1899.999175427747</v>
+        <v>2122.221397649969</v>
       </c>
       <c r="F127">
         <v>32</v>
@@ -4120,7 +4120,7 @@
         <v>6800</v>
       </c>
       <c r="E128">
-        <v>1725.396000824572</v>
+        <v>1860.316635745207</v>
       </c>
       <c r="F128">
         <v>32.0754716981132</v>
@@ -4140,7 +4140,7 @@
         <v>7200</v>
       </c>
       <c r="E129">
-        <v>1709.522984951556</v>
+        <v>1852.380127808699</v>
       </c>
       <c r="F129">
         <v>32</v>
@@ -4160,7 +4160,7 @@
         <v>7200</v>
       </c>
       <c r="E130">
-        <v>1601.189651618223</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F130">
         <v>32</v>
@@ -4180,7 +4180,7 @@
         <v>4800</v>
       </c>
       <c r="E131">
-        <v>1684.522984951556</v>
+        <v>1779.761080189651</v>
       </c>
       <c r="F131">
         <v>32</v>
@@ -4200,7 +4200,7 @@
         <v>4800</v>
       </c>
       <c r="E132">
-        <v>1684.522984951556</v>
+        <v>1779.761080189651</v>
       </c>
       <c r="F132">
         <v>32</v>
@@ -4220,7 +4220,7 @@
         <v>6000</v>
       </c>
       <c r="E133">
-        <v>1708.33250876108</v>
+        <v>1827.380127808699</v>
       </c>
       <c r="F133">
         <v>32.0855614973262</v>
@@ -4240,7 +4240,7 @@
         <v>4800</v>
       </c>
       <c r="E134">
-        <v>1732.142032570604</v>
+        <v>1827.380127808699</v>
       </c>
       <c r="F134">
         <v>32</v>
@@ -4260,7 +4260,7 @@
         <v>5600</v>
       </c>
       <c r="E135">
-        <v>1676.586477015048</v>
+        <v>1787.697588126159</v>
       </c>
       <c r="F135">
         <v>32</v>
@@ -4280,7 +4280,7 @@
         <v>4800</v>
       </c>
       <c r="E136">
-        <v>1721.427746856318</v>
+        <v>1816.665842094413</v>
       </c>
       <c r="F136">
         <v>32</v>
@@ -4300,7 +4300,7 @@
         <v>3600</v>
       </c>
       <c r="E137">
-        <v>1470.237270665842</v>
+        <v>1541.665842094413</v>
       </c>
       <c r="F137">
         <v>32.14285714285715</v>
@@ -4320,7 +4320,7 @@
         <v>1800</v>
       </c>
       <c r="E138">
-        <v>1744.046794475366</v>
+        <v>1779.761080189652</v>
       </c>
       <c r="F138">
         <v>32.14285714285715</v>
@@ -4340,7 +4340,7 @@
         <v>30000</v>
       </c>
       <c r="E139">
-        <v>2221.427746856318</v>
+        <v>2816.665842094413</v>
       </c>
       <c r="F139">
         <v>66.66666666666667</v>
@@ -4360,7 +4360,7 @@
         <v>6000</v>
       </c>
       <c r="E140">
-        <v>1505.951556380128</v>
+        <v>1624.999175427747</v>
       </c>
       <c r="F140">
         <v>32.0855614973262</v>
@@ -4380,7 +4380,7 @@
         <v>6000</v>
       </c>
       <c r="E141">
-        <v>1505.951556380128</v>
+        <v>1624.999175427747</v>
       </c>
       <c r="F141">
         <v>32.0855614973262</v>
@@ -4400,7 +4400,7 @@
         <v>6000</v>
       </c>
       <c r="E142">
-        <v>1589.284889713461</v>
+        <v>1708.33250876108</v>
       </c>
       <c r="F142">
         <v>32.0855614973262</v>
@@ -4420,7 +4420,7 @@
         <v>6000</v>
       </c>
       <c r="E143">
-        <v>1886.903937332509</v>
+        <v>2005.951556380128</v>
       </c>
       <c r="F143">
         <v>32.0855614973262</v>
@@ -4440,7 +4440,7 @@
         <v>4800</v>
       </c>
       <c r="E144">
-        <v>1458.33250876108</v>
+        <v>1553.570603999175</v>
       </c>
       <c r="F144">
         <v>32</v>
@@ -4460,7 +4460,7 @@
         <v>1800</v>
       </c>
       <c r="E145">
-        <v>257.1428571428572</v>
+        <v>385.7142857142858</v>
       </c>
       <c r="F145">
         <v>32.14285714285715</v>
@@ -4480,7 +4480,7 @@
         <v>7000</v>
       </c>
       <c r="E146">
-        <v>1871.030921459493</v>
+        <v>2009.919810348382</v>
       </c>
       <c r="F146">
         <v>32.11009174311926</v>
@@ -4500,7 +4500,7 @@
         <v>7000</v>
       </c>
       <c r="E147">
-        <v>1644.840445269017</v>
+        <v>1783.729334157905</v>
       </c>
       <c r="F147">
         <v>32.11009174311926</v>
@@ -4520,7 +4520,7 @@
         <v>7600</v>
       </c>
       <c r="E148">
-        <v>1787.697588126159</v>
+        <v>1938.49123891981</v>
       </c>
       <c r="F148">
         <v>32.06751054852321</v>
@@ -4540,7 +4540,7 @@
         <v>7200</v>
       </c>
       <c r="E149">
-        <v>1709.522984951556</v>
+        <v>1852.380127808699</v>
       </c>
       <c r="F149">
         <v>32</v>
@@ -4560,7 +4560,7 @@
         <v>4800</v>
       </c>
       <c r="E150">
-        <v>1613.094413522985</v>
+        <v>1708.33250876108</v>
       </c>
       <c r="F150">
         <v>32</v>
@@ -4580,7 +4580,7 @@
         <v>8400</v>
       </c>
       <c r="E151">
-        <v>1959.522984951556</v>
+        <v>2126.189651618223</v>
       </c>
       <c r="F151">
         <v>32.06106870229008</v>
@@ -4600,7 +4600,7 @@
         <v>6000</v>
       </c>
       <c r="E152">
-        <v>1783.729334157905</v>
+        <v>1902.776953205524</v>
       </c>
       <c r="F152">
         <v>32.0855614973262</v>
@@ -4620,7 +4620,7 @@
         <v>8800</v>
       </c>
       <c r="E153">
-        <v>1609.126159554731</v>
+        <v>1783.729334157905</v>
       </c>
       <c r="F153">
         <v>32</v>
@@ -4640,7 +4640,7 @@
         <v>8000</v>
       </c>
       <c r="E154">
-        <v>1546.824572253144</v>
+        <v>1705.554730983302</v>
       </c>
       <c r="F154">
         <v>32</v>
@@ -4660,7 +4660,7 @@
         <v>8000</v>
       </c>
       <c r="E155">
-        <v>1706.348381776953</v>
+        <v>1865.078540507112</v>
       </c>
       <c r="F155">
         <v>32</v>
@@ -4680,7 +4680,7 @@
         <v>13200</v>
       </c>
       <c r="E156">
-        <v>2161.903937332509</v>
+        <v>2423.808699237271</v>
       </c>
       <c r="F156">
         <v>32.03883495145631</v>
@@ -4700,7 +4700,7 @@
         <v>7200</v>
       </c>
       <c r="E157">
-        <v>1590.475365903937</v>
+        <v>1733.33250876108</v>
       </c>
       <c r="F157">
         <v>32</v>
@@ -4720,7 +4720,7 @@
         <v>7200</v>
       </c>
       <c r="E158">
-        <v>1708.33250876108</v>
+        <v>1851.189651618223</v>
       </c>
       <c r="F158">
         <v>32</v>
@@ -4740,7 +4740,7 @@
         <v>9200</v>
       </c>
       <c r="E159">
-        <v>1783.729334157905</v>
+        <v>1966.269016697588</v>
       </c>
       <c r="F159">
         <v>32.05574912891986</v>
@@ -4760,7 +4760,7 @@
         <v>3600</v>
       </c>
       <c r="E160">
-        <v>1589.284889713461</v>
+        <v>1660.713461142032</v>
       </c>
       <c r="F160">
         <v>32.14285714285715</v>
@@ -4780,7 +4780,7 @@
         <v>1800</v>
       </c>
       <c r="E161">
-        <v>1745.237270665842</v>
+        <v>1780.951556380128</v>
       </c>
       <c r="F161">
         <v>32.14285714285715</v>
@@ -4800,7 +4800,7 @@
         <v>4800</v>
       </c>
       <c r="E162">
-        <v>1589.284889713461</v>
+        <v>1684.522984951556</v>
       </c>
       <c r="F162">
         <v>32</v>
@@ -4820,7 +4820,7 @@
         <v>6000</v>
       </c>
       <c r="E163">
-        <v>1803.570603999175</v>
+        <v>1922.618223046794</v>
       </c>
       <c r="F163">
         <v>32.0855614973262</v>
@@ -4840,7 +4840,7 @@
         <v>6000</v>
       </c>
       <c r="E164">
-        <v>1851.189651618223</v>
+        <v>1970.237270665842</v>
       </c>
       <c r="F164">
         <v>32.0855614973262</v>
@@ -4860,7 +4860,7 @@
         <v>4000</v>
       </c>
       <c r="E165">
-        <v>1562.69758812616</v>
+        <v>1642.062667491239</v>
       </c>
       <c r="F165">
         <v>32</v>
@@ -4880,7 +4880,7 @@
         <v>7600</v>
       </c>
       <c r="E166">
-        <v>1827.380127808699</v>
+        <v>1978.17377860235</v>
       </c>
       <c r="F166">
         <v>32.06751054852321</v>
@@ -4900,7 +4900,7 @@
         <v>2400</v>
       </c>
       <c r="E167">
-        <v>1517.85631828489</v>
+        <v>1565.475365903937</v>
       </c>
       <c r="F167">
         <v>32</v>
@@ -4920,7 +4920,7 @@
         <v>4800</v>
       </c>
       <c r="E168">
-        <v>1685.713461142032</v>
+        <v>1780.951556380128</v>
       </c>
       <c r="F168">
         <v>32</v>
@@ -4940,7 +4940,7 @@
         <v>4800</v>
       </c>
       <c r="E169">
-        <v>1642.062667491239</v>
+        <v>1737.300762729334</v>
       </c>
       <c r="F169">
         <v>32</v>
@@ -4960,7 +4960,7 @@
         <v>2400</v>
       </c>
       <c r="E170">
-        <v>1488.094413522985</v>
+        <v>1535.713461142033</v>
       </c>
       <c r="F170">
         <v>32</v>
@@ -4980,7 +4980,7 @@
         <v>6000</v>
       </c>
       <c r="E171">
-        <v>1577.380127808699</v>
+        <v>1696.427746856318</v>
       </c>
       <c r="F171">
         <v>32.0855614973262</v>
@@ -5000,7 +5000,7 @@
         <v>6000</v>
       </c>
       <c r="E172">
-        <v>1624.999175427747</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F172">
         <v>32.0855614973262</v>
@@ -5020,7 +5020,7 @@
         <v>8000</v>
       </c>
       <c r="E173">
-        <v>1624.999175427747</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F173">
         <v>32</v>
@@ -5040,7 +5040,7 @@
         <v>8000</v>
       </c>
       <c r="E174">
-        <v>2045.634096062667</v>
+        <v>2204.364254792826</v>
       </c>
       <c r="F174">
         <v>32</v>
@@ -5060,7 +5060,7 @@
         <v>4800</v>
       </c>
       <c r="E175">
-        <v>1505.951556380128</v>
+        <v>1601.189651618223</v>
       </c>
       <c r="F175">
         <v>32</v>
@@ -5080,7 +5080,7 @@
         <v>600</v>
       </c>
       <c r="E176">
-        <v>1470.237270665842</v>
+        <v>1482.142032570604</v>
       </c>
       <c r="F176">
         <v>33.33333333333334</v>
@@ -5100,7 +5100,7 @@
         <v>2000</v>
       </c>
       <c r="E177">
-        <v>1450.396000824572</v>
+        <v>1490.078540507112</v>
       </c>
       <c r="F177">
         <v>32.25806451612903</v>
@@ -5120,7 +5120,7 @@
         <v>3600</v>
       </c>
       <c r="E178">
-        <v>1482.142032570604</v>
+        <v>1553.570603999175</v>
       </c>
       <c r="F178">
         <v>32.14285714285715</v>
@@ -5140,7 +5140,7 @@
         <v>7200</v>
       </c>
       <c r="E179">
-        <v>1499.999175427747</v>
+        <v>1642.85631828489</v>
       </c>
       <c r="F179">
         <v>32</v>
@@ -5160,7 +5160,7 @@
         <v>9000</v>
       </c>
       <c r="E180">
-        <v>2049.602350030921</v>
+        <v>2228.17377860235</v>
       </c>
       <c r="F180">
         <v>32.02846975088968</v>
@@ -5180,7 +5180,7 @@
         <v>6000</v>
       </c>
       <c r="E181">
-        <v>1906.745207173778</v>
+        <v>2025.792826221397</v>
       </c>
       <c r="F181">
         <v>32.0855614973262</v>
@@ -5200,7 +5200,7 @@
         <v>3600</v>
       </c>
       <c r="E182">
-        <v>1601.189651618223</v>
+        <v>1672.618223046794</v>
       </c>
       <c r="F182">
         <v>32.14285714285715</v>
@@ -5220,7 +5220,7 @@
         <v>9000</v>
       </c>
       <c r="E183">
-        <v>1823.411873840445</v>
+        <v>2001.983302411874</v>
       </c>
       <c r="F183">
         <v>32.02846975088968</v>
@@ -5240,7 +5240,7 @@
         <v>9600</v>
       </c>
       <c r="E184">
-        <v>1978.17377860235</v>
+        <v>2168.64996907854</v>
       </c>
       <c r="F184">
         <v>32</v>
@@ -5260,7 +5260,7 @@
         <v>6000</v>
       </c>
       <c r="E185">
-        <v>1709.522984951556</v>
+        <v>1828.570603999175</v>
       </c>
       <c r="F185">
         <v>32.0855614973262</v>
@@ -5280,7 +5280,7 @@
         <v>9200</v>
       </c>
       <c r="E186">
-        <v>1892.062667491239</v>
+        <v>2074.602350030921</v>
       </c>
       <c r="F186">
         <v>32.05574912891986</v>
@@ -5300,7 +5300,7 @@
         <v>7200</v>
       </c>
       <c r="E187">
-        <v>1852.380127808699</v>
+        <v>1995.237270665842</v>
       </c>
       <c r="F187">
         <v>32</v>
@@ -5320,7 +5320,7 @@
         <v>9600</v>
       </c>
       <c r="E188">
-        <v>2149.999175427747</v>
+        <v>2340.475365903937</v>
       </c>
       <c r="F188">
         <v>32</v>
@@ -5340,7 +5340,7 @@
         <v>8000</v>
       </c>
       <c r="E189">
-        <v>1942.459492888064</v>
+        <v>2101.189651618223</v>
       </c>
       <c r="F189">
         <v>32</v>
@@ -5360,7 +5360,7 @@
         <v>9600</v>
       </c>
       <c r="E190">
-        <v>1737.300762729334</v>
+        <v>1927.776953205524</v>
       </c>
       <c r="F190">
         <v>32</v>
@@ -5380,7 +5380,7 @@
         <v>9000</v>
       </c>
       <c r="E191">
-        <v>1589.284889713461</v>
+        <v>1767.85631828489</v>
       </c>
       <c r="F191">
         <v>32.02846975088968</v>
@@ -5400,7 +5400,7 @@
         <v>11200</v>
       </c>
       <c r="E192">
-        <v>2005.951556380128</v>
+        <v>2228.17377860235</v>
       </c>
       <c r="F192">
         <v>32</v>
@@ -5420,7 +5420,7 @@
         <v>6000</v>
       </c>
       <c r="E193">
-        <v>1720.237270665842</v>
+        <v>1839.284889713461</v>
       </c>
       <c r="F193">
         <v>32.0855614973262</v>
@@ -5440,7 +5440,7 @@
         <v>7200</v>
       </c>
       <c r="E194">
-        <v>1946.427746856318</v>
+        <v>2089.284889713461</v>
       </c>
       <c r="F194">
         <v>32</v>
@@ -5460,7 +5460,7 @@
         <v>6000</v>
       </c>
       <c r="E195">
-        <v>1708.33250876108</v>
+        <v>1827.380127808699</v>
       </c>
       <c r="F195">
         <v>32.0855614973262</v>
@@ -5480,7 +5480,7 @@
         <v>4000</v>
       </c>
       <c r="E196">
-        <v>1562.69758812616</v>
+        <v>1642.062667491239</v>
       </c>
       <c r="F196">
         <v>32</v>
@@ -5500,7 +5500,7 @@
         <v>9600</v>
       </c>
       <c r="E197">
-        <v>2017.85631828489</v>
+        <v>2208.33250876108</v>
       </c>
       <c r="F197">
         <v>32</v>
@@ -5520,7 +5520,7 @@
         <v>6000</v>
       </c>
       <c r="E198">
-        <v>1661.903937332509</v>
+        <v>1780.951556380128</v>
       </c>
       <c r="F198">
         <v>32.0855614973262</v>
@@ -5540,7 +5540,7 @@
         <v>6400</v>
       </c>
       <c r="E199">
-        <v>1704.364254792826</v>
+        <v>1831.348381776953</v>
       </c>
       <c r="F199">
         <v>32</v>
@@ -5560,7 +5560,7 @@
         <v>4800</v>
       </c>
       <c r="E200">
-        <v>1684.522984951556</v>
+        <v>1779.761080189651</v>
       </c>
       <c r="F200">
         <v>32</v>
@@ -5580,7 +5580,7 @@
         <v>4800</v>
       </c>
       <c r="E201">
-        <v>1685.713461142032</v>
+        <v>1780.951556380128</v>
       </c>
       <c r="F201">
         <v>32</v>
@@ -5600,7 +5600,7 @@
         <v>8000</v>
       </c>
       <c r="E202">
-        <v>1736.110286538858</v>
+        <v>1894.840445269017</v>
       </c>
       <c r="F202">
         <v>32</v>
@@ -5620,7 +5620,7 @@
         <v>6000</v>
       </c>
       <c r="E203">
-        <v>1736.110286538858</v>
+        <v>1894.840445269017</v>
       </c>
       <c r="F203">
         <v>32.0855614973262</v>
@@ -5640,7 +5640,7 @@
         <v>6000</v>
       </c>
       <c r="E204">
-        <v>1744.046794475366</v>
+        <v>1863.094413522985</v>
       </c>
       <c r="F204">
         <v>32.0855614973262</v>
@@ -5660,7 +5660,7 @@
         <v>10000</v>
       </c>
       <c r="E205">
-        <v>1744.046794475366</v>
+        <v>1863.094413522985</v>
       </c>
       <c r="F205">
         <v>32.05128205128205</v>
@@ -5680,7 +5680,7 @@
         <v>10000</v>
       </c>
       <c r="E206">
-        <v>1656.745207173778</v>
+        <v>1855.157905586477</v>
       </c>
       <c r="F206">
         <v>32.05128205128205</v>
@@ -5700,7 +5700,7 @@
         <v>3600</v>
       </c>
       <c r="E207">
-        <v>1470.237270665842</v>
+        <v>1541.665842094413</v>
       </c>
       <c r="F207">
         <v>32.14285714285715</v>
@@ -5720,7 +5720,7 @@
         <v>8400</v>
       </c>
       <c r="E208">
-        <v>1648.808699237271</v>
+        <v>1815.475365903937</v>
       </c>
       <c r="F208">
         <v>32.06106870229008</v>
@@ -5740,7 +5740,7 @@
         <v>7200</v>
       </c>
       <c r="E209">
-        <v>1541.665842094414</v>
+        <v>1684.522984951557</v>
       </c>
       <c r="F209">
         <v>32</v>
@@ -5760,7 +5760,7 @@
         <v>7200</v>
       </c>
       <c r="E210">
-        <v>1601.189651618223</v>
+        <v>1744.046794475366</v>
       </c>
       <c r="F210">
         <v>32</v>
@@ -5780,7 +5780,7 @@
         <v>11000</v>
       </c>
       <c r="E211">
-        <v>2041.665842094413</v>
+        <v>2259.919810348381</v>
       </c>
       <c r="F211">
         <v>32.06997084548105</v>
@@ -5800,7 +5800,7 @@
         <v>11600</v>
       </c>
       <c r="E212">
-        <v>2208.33250876108</v>
+        <v>2438.49123891981</v>
       </c>
       <c r="F212">
         <v>32.04419889502763</v>
@@ -5820,7 +5820,7 @@
         <v>9600</v>
       </c>
       <c r="E213">
-        <v>2090.475365903937</v>
+        <v>2280.951556380127</v>
       </c>
       <c r="F213">
         <v>32</v>
@@ -5840,7 +5840,7 @@
         <v>6000</v>
       </c>
       <c r="E214">
-        <v>1780.951556380128</v>
+        <v>1899.999175427747</v>
       </c>
       <c r="F214">
         <v>32.0855614973262</v>
@@ -5860,7 +5860,7 @@
         <v>11200</v>
       </c>
       <c r="E215">
-        <v>2114.284889713461</v>
+        <v>2336.507111935683</v>
       </c>
       <c r="F215">
         <v>32</v>
@@ -5880,7 +5880,7 @@
         <v>10800</v>
       </c>
       <c r="E216">
-        <v>2364.284889713461</v>
+        <v>2578.570603999175</v>
       </c>
       <c r="F216">
         <v>32.04747774480713</v>
@@ -5900,7 +5900,7 @@
         <v>10000</v>
       </c>
       <c r="E217">
-        <v>2140.872191300763</v>
+        <v>2339.284889713461</v>
       </c>
       <c r="F217">
         <v>32.05128205128205</v>
@@ -5920,7 +5920,7 @@
         <v>7200</v>
       </c>
       <c r="E218">
-        <v>1732.142032570604</v>
+        <v>1874.999175427747</v>
       </c>
       <c r="F218">
         <v>32</v>
@@ -5940,7 +5940,7 @@
         <v>6000</v>
       </c>
       <c r="E219">
-        <v>1708.33250876108</v>
+        <v>1827.380127808699</v>
       </c>
       <c r="F219">
         <v>32.0855614973262</v>
@@ -5960,7 +5960,7 @@
         <v>13200</v>
       </c>
       <c r="E220">
-        <v>2267.856318284889</v>
+        <v>2529.761080189651</v>
       </c>
       <c r="F220">
         <v>32.03883495145631</v>
@@ -5980,7 +5980,7 @@
         <v>8000</v>
       </c>
       <c r="E221">
-        <v>1878.967429396001</v>
+        <v>2037.697588126159</v>
       </c>
       <c r="F221">
         <v>32</v>
@@ -6000,7 +6000,7 @@
         <v>12000</v>
       </c>
       <c r="E222">
-        <v>1721.427746856318</v>
+        <v>1959.522984951556</v>
       </c>
       <c r="F222">
         <v>32</v>
@@ -6020,7 +6020,7 @@
         <v>8400</v>
       </c>
       <c r="E223">
-        <v>2113.094413522985</v>
+        <v>2279.761080189651</v>
       </c>
       <c r="F223">
         <v>32.06106870229008</v>
@@ -6040,7 +6040,7 @@
         <v>7200</v>
       </c>
       <c r="E224">
-        <v>1648.808699237271</v>
+        <v>1791.665842094413</v>
       </c>
       <c r="F224">
         <v>32</v>
@@ -6060,7 +6060,7 @@
         <v>10000</v>
       </c>
       <c r="E225">
-        <v>1906.745207173778</v>
+        <v>2105.157905586477</v>
       </c>
       <c r="F225">
         <v>32.05128205128205</v>
@@ -6080,7 +6080,7 @@
         <v>7200</v>
       </c>
       <c r="E226">
-        <v>1803.570603999175</v>
+        <v>1946.427746856318</v>
       </c>
       <c r="F226">
         <v>32</v>
@@ -6100,7 +6100,7 @@
         <v>5000</v>
       </c>
       <c r="E227">
-        <v>1521.824572253144</v>
+        <v>1621.030921459493</v>
       </c>
       <c r="F227">
         <v>11.11111111111111</v>
@@ -6120,7 +6120,7 @@
         <v>8000</v>
       </c>
       <c r="E228">
-        <v>2009.919810348382</v>
+        <v>2168.64996907854</v>
       </c>
       <c r="F228">
         <v>32</v>
@@ -6140,7 +6140,7 @@
         <v>4000</v>
       </c>
       <c r="E229">
-        <v>1626.189651618223</v>
+        <v>1705.554730983302</v>
       </c>
       <c r="F229">
         <v>32</v>
@@ -6160,7 +6160,7 @@
         <v>5000</v>
       </c>
       <c r="E230">
-        <v>1775.792826221397</v>
+        <v>1874.999175427747</v>
       </c>
       <c r="F230">
         <v>32.05128205128205</v>
@@ -6180,7 +6180,7 @@
         <v>11600</v>
       </c>
       <c r="E231">
-        <v>2248.01504844362</v>
+        <v>2478.17377860235</v>
       </c>
       <c r="F231">
         <v>32.04419889502763</v>
@@ -6200,7 +6200,7 @@
         <v>4800</v>
       </c>
       <c r="E232">
-        <v>2001.983302411874</v>
+        <v>2097.221397649969</v>
       </c>
       <c r="F232">
         <v>32</v>
@@ -6220,7 +6220,7 @@
         <v>4800</v>
       </c>
       <c r="E233">
-        <v>2001.983302411874</v>
+        <v>2097.221397649969</v>
       </c>
       <c r="F233">
         <v>32</v>
@@ -6240,7 +6240,7 @@
         <v>14400</v>
       </c>
       <c r="E234">
-        <v>2007.142032570604</v>
+        <v>2292.856318284889</v>
       </c>
       <c r="F234">
         <v>32</v>
@@ -6260,7 +6260,7 @@
         <v>8400</v>
       </c>
       <c r="E235">
-        <v>1902.776953205524</v>
+        <v>2069.443619872191</v>
       </c>
       <c r="F235">
         <v>32.06106870229008</v>
@@ -6280,7 +6280,7 @@
         <v>5000</v>
       </c>
       <c r="E236">
-        <v>2005.951556380128</v>
+        <v>2105.157905586477</v>
       </c>
       <c r="F236">
         <v>32.05128205128205</v>
@@ -6300,7 +6300,7 @@
         <v>30000</v>
       </c>
       <c r="E237">
-        <v>2257.142032570604</v>
+        <v>2852.380127808699</v>
       </c>
       <c r="F237">
         <v>66.66666666666667</v>
@@ -6320,7 +6320,7 @@
         <v>10000</v>
       </c>
       <c r="E238">
-        <v>1934.522984951556</v>
+        <v>2132.935683364255</v>
       </c>
       <c r="F238">
         <v>32.05128205128205</v>
@@ -6340,7 +6340,7 @@
         <v>8000</v>
       </c>
       <c r="E239">
-        <v>1819.443619872191</v>
+        <v>1978.17377860235</v>
       </c>
       <c r="F239">
         <v>32</v>
@@ -6360,7 +6360,7 @@
         <v>9000</v>
       </c>
       <c r="E240">
-        <v>1922.618223046794</v>
+        <v>2101.189651618223</v>
       </c>
       <c r="F240">
         <v>32.02846975088968</v>
@@ -6380,7 +6380,7 @@
         <v>12000</v>
       </c>
       <c r="E241">
-        <v>1922.618223046794</v>
+        <v>2101.189651618223</v>
       </c>
       <c r="F241">
         <v>32</v>
@@ -6400,7 +6400,7 @@
         <v>12000</v>
       </c>
       <c r="E242">
-        <v>1894.840445269017</v>
+        <v>2132.935683364255</v>
       </c>
       <c r="F242">
         <v>32</v>
@@ -6420,7 +6420,7 @@
         <v>7200</v>
       </c>
       <c r="E243">
-        <v>1624.999175427747</v>
+        <v>1767.85631828489</v>
       </c>
       <c r="F243">
         <v>32</v>
@@ -6440,7 +6440,7 @@
         <v>14400</v>
       </c>
       <c r="E244">
-        <v>1642.85631828489</v>
+        <v>1928.570603999176</v>
       </c>
       <c r="F244">
         <v>32</v>
@@ -6460,7 +6460,7 @@
         <v>7200</v>
       </c>
       <c r="E245">
-        <v>1541.665842094414</v>
+        <v>1684.522984951557</v>
       </c>
       <c r="F245">
         <v>32</v>
@@ -6480,7 +6480,7 @@
         <v>11000</v>
       </c>
       <c r="E246">
-        <v>2267.856318284889</v>
+        <v>2486.110286538858</v>
       </c>
       <c r="F246">
         <v>32.06997084548105</v>
@@ -6500,7 +6500,7 @@
         <v>8400</v>
       </c>
       <c r="E247">
-        <v>1672.618223046794</v>
+        <v>1839.284889713461</v>
       </c>
       <c r="F247">
         <v>32.06106870229008</v>
@@ -6520,7 +6520,7 @@
         <v>13600</v>
       </c>
       <c r="E248">
-        <v>2385.988186416758</v>
+        <v>2635.072435501007</v>
       </c>
       <c r="F248">
         <v>32</v>
@@ -6540,7 +6540,7 @@
         <v>6000</v>
       </c>
       <c r="E249">
-        <v>1590.475365903937</v>
+        <v>1709.522984951556</v>
       </c>
       <c r="F249">
         <v>32.0855614973262</v>
@@ -6560,7 +6560,7 @@
         <v>10800</v>
       </c>
       <c r="E250">
-        <v>2304.761080189651</v>
+        <v>2519.046794475365</v>
       </c>
       <c r="F250">
         <v>32.04747774480713</v>
@@ -6580,7 +6580,7 @@
         <v>8000</v>
       </c>
       <c r="E251">
-        <v>1939.681715110286</v>
+        <v>2098.411873840445</v>
       </c>
       <c r="F251">
         <v>32</v>
@@ -6600,7 +6600,7 @@
         <v>12000</v>
       </c>
       <c r="E252">
-        <v>2566.574267002838</v>
+        <v>2786.354486783058</v>
       </c>
       <c r="F252">
         <v>32</v>
@@ -6620,7 +6620,7 @@
         <v>12000</v>
       </c>
       <c r="E253">
-        <v>2360.347160775732</v>
+        <v>2580.127380555952</v>
       </c>
       <c r="F253">
         <v>32</v>
@@ -6640,7 +6640,7 @@
         <v>9200</v>
       </c>
       <c r="E254">
-        <v>1843.253143681715</v>
+        <v>2025.792826221397</v>
       </c>
       <c r="F254">
         <v>32.05574912891986</v>
@@ -6660,7 +6660,7 @@
         <v>8000</v>
       </c>
       <c r="E255">
-        <v>1867.062667491239</v>
+        <v>2025.792826221397</v>
       </c>
       <c r="F255">
         <v>32</v>
@@ -6680,7 +6680,7 @@
         <v>14400</v>
       </c>
       <c r="E256">
-        <v>1767.85631828489</v>
+        <v>2053.570603999175</v>
       </c>
       <c r="F256">
         <v>32</v>
@@ -6700,7 +6700,7 @@
         <v>15200</v>
       </c>
       <c r="E257">
-        <v>2415.292215720787</v>
+        <v>2693.680494109065</v>
       </c>
       <c r="F257">
         <v>33.77777777777778</v>
@@ -6720,7 +6720,7 @@
         <v>15000</v>
       </c>
       <c r="E258">
-        <v>1888.094413522985</v>
+        <v>2185.713461142032</v>
       </c>
       <c r="F258">
         <v>33.33333333333334</v>
@@ -6740,7 +6740,7 @@
         <v>14400</v>
       </c>
       <c r="E259">
-        <v>2089.284889713461</v>
+        <v>2374.999175427747</v>
       </c>
       <c r="F259">
         <v>32</v>
@@ -6760,7 +6760,7 @@
         <v>10000</v>
       </c>
       <c r="E260">
-        <v>2077.380127808699</v>
+        <v>2275.792826221397</v>
       </c>
       <c r="F260">
         <v>32.05128205128205</v>
@@ -6780,7 +6780,7 @@
         <v>10000</v>
       </c>
       <c r="E261">
-        <v>1799.602350030921</v>
+        <v>1998.01504844362</v>
       </c>
       <c r="F261">
         <v>32.05128205128205</v>
@@ -6800,7 +6800,7 @@
         <v>7200</v>
       </c>
       <c r="E262">
-        <v>1799.602350030921</v>
+        <v>1998.01504844362</v>
       </c>
       <c r="F262">
         <v>32</v>
@@ -6820,7 +6820,7 @@
         <v>14400</v>
       </c>
       <c r="E263">
-        <v>1769.046794475366</v>
+        <v>2054.761080189652</v>
       </c>
       <c r="F263">
         <v>32</v>
@@ -6840,7 +6840,7 @@
         <v>9600</v>
       </c>
       <c r="E264">
-        <v>2303.570603999175</v>
+        <v>2494.046794475365</v>
       </c>
       <c r="F264">
         <v>32</v>
@@ -6860,7 +6860,7 @@
         <v>10000</v>
       </c>
       <c r="E265">
-        <v>2208.33250876108</v>
+        <v>2406.745207173778</v>
       </c>
       <c r="F265">
         <v>32.05128205128205</v>
@@ -6880,7 +6880,7 @@
         <v>5000</v>
       </c>
       <c r="E266">
-        <v>1775.792826221397</v>
+        <v>1874.999175427747</v>
       </c>
       <c r="F266">
         <v>32.05128205128205</v>
@@ -6900,7 +6900,7 @@
         <v>13600</v>
       </c>
       <c r="E267">
-        <v>2488.55228898086</v>
+        <v>2737.63653806511</v>
       </c>
       <c r="F267">
         <v>32</v>
@@ -6920,7 +6920,7 @@
         <v>7200</v>
       </c>
       <c r="E268">
-        <v>2232.142032570604</v>
+        <v>2374.999175427747</v>
       </c>
       <c r="F268">
         <v>32</v>
@@ -6940,7 +6940,7 @@
         <v>7200</v>
       </c>
       <c r="E269">
-        <v>1911.903937332509</v>
+        <v>2054.761080189651</v>
       </c>
       <c r="F269">
         <v>32</v>
@@ -6960,7 +6960,7 @@
         <v>4000</v>
       </c>
       <c r="E270">
-        <v>1740.078540507112</v>
+        <v>1819.443619872191</v>
       </c>
       <c r="F270">
         <v>32</v>
@@ -6980,7 +6980,7 @@
         <v>14400</v>
       </c>
       <c r="E271">
-        <v>2053.570603999175</v>
+        <v>2339.284889713461</v>
       </c>
       <c r="F271">
         <v>32</v>
@@ -7000,7 +7000,7 @@
         <v>4800</v>
       </c>
       <c r="E272">
-        <v>1894.840445269017</v>
+        <v>1990.078540507112</v>
       </c>
       <c r="F272">
         <v>32</v>
@@ -7020,7 +7020,7 @@
         <v>12000</v>
       </c>
       <c r="E273">
-        <v>1974.205524634096</v>
+        <v>2212.300762729334</v>
       </c>
       <c r="F273">
         <v>32</v>
@@ -7040,7 +7040,7 @@
         <v>7200</v>
       </c>
       <c r="E274">
-        <v>2232.142032570604</v>
+        <v>2374.999175427747</v>
       </c>
       <c r="F274">
         <v>32</v>
@@ -7060,7 +7060,7 @@
         <v>15000</v>
       </c>
       <c r="E275">
-        <v>2185.713461142032</v>
+        <v>2483.33250876108</v>
       </c>
       <c r="F275">
         <v>33.33333333333334</v>
@@ -7080,7 +7080,7 @@
         <v>10000</v>
       </c>
       <c r="E276">
-        <v>2017.85631828489</v>
+        <v>2216.269016697588</v>
       </c>
       <c r="F276">
         <v>32.05128205128205</v>
@@ -7100,7 +7100,7 @@
         <v>12000</v>
       </c>
       <c r="E277">
-        <v>2160.713461142032</v>
+        <v>2398.808699237271</v>
       </c>
       <c r="F277">
         <v>32</v>
@@ -7120,7 +7120,7 @@
         <v>14000</v>
       </c>
       <c r="E278">
-        <v>2160.713461142032</v>
+        <v>2398.808699237271</v>
       </c>
       <c r="F278">
         <v>32.03661327231121</v>
@@ -7140,7 +7140,7 @@
         <v>14000</v>
       </c>
       <c r="E279">
-        <v>2172.618223046794</v>
+        <v>2450.396000824572</v>
       </c>
       <c r="F279">
         <v>32.03661327231121</v>
@@ -7160,7 +7160,7 @@
         <v>14400</v>
       </c>
       <c r="E280">
-        <v>2601.582116296402</v>
+        <v>2846.480075480075</v>
       </c>
       <c r="F280">
         <v>32</v>
@@ -7180,7 +7180,7 @@
         <v>9600</v>
       </c>
       <c r="E281">
-        <v>1648.808699237271</v>
+        <v>1839.284889713461</v>
       </c>
       <c r="F281">
         <v>32</v>
@@ -7200,7 +7200,7 @@
         <v>16400</v>
       </c>
       <c r="E282">
-        <v>1724.205524634096</v>
+        <v>2049.602350030921</v>
       </c>
       <c r="F282">
         <v>36.44444444444444</v>
@@ -7220,7 +7220,7 @@
         <v>13000</v>
       </c>
       <c r="E283">
-        <v>2495.878296306867</v>
+        <v>2733.973534402106</v>
       </c>
       <c r="F283">
         <v>32.01970443349754</v>
@@ -7240,7 +7240,7 @@
         <v>14400</v>
       </c>
       <c r="E284">
-        <v>2109.126159554731</v>
+        <v>2394.840445269017</v>
       </c>
       <c r="F284">
         <v>32</v>
@@ -7260,7 +7260,7 @@
         <v>13000</v>
       </c>
       <c r="E285">
-        <v>1859.126159554731</v>
+        <v>2117.062667491239</v>
       </c>
       <c r="F285">
         <v>32.01970443349754</v>
@@ -7280,7 +7280,7 @@
         <v>15600</v>
       </c>
       <c r="E286">
-        <v>2649.201163915449</v>
+        <v>2914.507286364429</v>
       </c>
       <c r="F286">
         <v>34.66666666666666</v>
@@ -7300,7 +7300,7 @@
         <v>7200</v>
       </c>
       <c r="E287">
-        <v>1733.33250876108</v>
+        <v>1876.189651618223</v>
       </c>
       <c r="F287">
         <v>32</v>
@@ -7320,7 +7320,7 @@
         <v>12000</v>
       </c>
       <c r="E288">
-        <v>2511.629212057783</v>
+        <v>2731.409431838003</v>
       </c>
       <c r="F288">
         <v>32</v>
@@ -7340,7 +7340,7 @@
         <v>10000</v>
       </c>
       <c r="E289">
-        <v>2138.094413522985</v>
+        <v>2336.507111935683</v>
       </c>
       <c r="F289">
         <v>32.05128205128205</v>
@@ -7360,7 +7360,7 @@
         <v>20000</v>
       </c>
       <c r="E290">
-        <v>2057.538857967429</v>
+        <v>2454.364254792826</v>
       </c>
       <c r="F290">
         <v>44.44444444444444</v>
@@ -7380,7 +7380,7 @@
         <v>14000</v>
       </c>
       <c r="E291">
-        <v>2598.180755752184</v>
+        <v>2836.275993847422</v>
       </c>
       <c r="F291">
         <v>32.03661327231121</v>
@@ -7400,7 +7400,7 @@
         <v>14400</v>
       </c>
       <c r="E292">
-        <v>2053.570603999175</v>
+        <v>2339.284889713461</v>
       </c>
       <c r="F292">
         <v>32</v>
@@ -7420,7 +7420,7 @@
         <v>13200</v>
       </c>
       <c r="E293">
-        <v>1922.618223046794</v>
+        <v>2184.522984951556</v>
       </c>
       <c r="F293">
         <v>32.03883495145631</v>
@@ -7440,7 +7440,7 @@
         <v>11200</v>
       </c>
       <c r="E294">
-        <v>2065.475365903937</v>
+        <v>2287.697588126159</v>
       </c>
       <c r="F294">
         <v>32</v>
@@ -7460,7 +7460,7 @@
         <v>10000</v>
       </c>
       <c r="E295">
-        <v>2065.475365903937</v>
+        <v>2263.888064316635</v>
       </c>
       <c r="F295">
         <v>32.05128205128205</v>
@@ -7480,7 +7480,7 @@
         <v>10000</v>
       </c>
       <c r="E296">
-        <v>1787.697588126159</v>
+        <v>1986.110286538858</v>
       </c>
       <c r="F296">
         <v>32.05128205128205</v>
@@ -7500,7 +7500,7 @@
         <v>28800</v>
       </c>
       <c r="E297">
-        <v>2196.427746856318</v>
+        <v>2767.856318284889</v>
       </c>
       <c r="F297">
         <v>64</v>
@@ -7520,7 +7520,7 @@
         <v>14400</v>
       </c>
       <c r="E298">
-        <v>1791.665842094413</v>
+        <v>2077.380127808699</v>
       </c>
       <c r="F298">
         <v>32</v>
@@ -7540,7 +7540,7 @@
         <v>14400</v>
       </c>
       <c r="E299">
-        <v>1767.85631828489</v>
+        <v>2053.570603999175</v>
       </c>
       <c r="F299">
         <v>32</v>
@@ -7560,7 +7560,7 @@
         <v>14400</v>
       </c>
       <c r="E300">
-        <v>1767.85631828489</v>
+        <v>2053.570603999175</v>
       </c>
       <c r="F300">
         <v>32</v>
@@ -7580,7 +7580,7 @@
         <v>9200</v>
       </c>
       <c r="E301">
-        <v>1890.872191300763</v>
+        <v>2073.411873840445</v>
       </c>
       <c r="F301">
         <v>32.05574912891986</v>
@@ -7600,7 +7600,7 @@
         <v>14400</v>
       </c>
       <c r="E302">
-        <v>2054.761080189651</v>
+        <v>2340.475365903937</v>
       </c>
       <c r="F302">
         <v>32</v>
@@ -7620,7 +7620,7 @@
         <v>10800</v>
       </c>
       <c r="E303">
-        <v>2488.55228898086</v>
+        <v>2686.354486783058</v>
       </c>
       <c r="F303">
         <v>32.04747774480713</v>
@@ -7640,7 +7640,7 @@
         <v>12000</v>
       </c>
       <c r="E304">
-        <v>2422.618223046794</v>
+        <v>2642.398442827014</v>
       </c>
       <c r="F304">
         <v>32</v>
@@ -7660,7 +7660,7 @@
         <v>5000</v>
       </c>
       <c r="E305">
-        <v>2295.634096062667</v>
+        <v>2394.840445269017</v>
       </c>
       <c r="F305">
         <v>32.05128205128205</v>
@@ -7680,7 +7680,7 @@
         <v>15600</v>
       </c>
       <c r="E306">
-        <v>2744.439259153545</v>
+        <v>3009.745381602525</v>
       </c>
       <c r="F306">
         <v>34.66666666666666</v>
@@ -7700,7 +7700,7 @@
         <v>6000</v>
       </c>
       <c r="E307">
-        <v>1803.570603999175</v>
+        <v>1922.618223046794</v>
       </c>
       <c r="F307">
         <v>32.0855614973262</v>
@@ -7720,7 +7720,7 @@
         <v>14400</v>
       </c>
       <c r="E308">
-        <v>2077.380127808699</v>
+        <v>2363.094413522985</v>
       </c>
       <c r="F308">
         <v>32</v>
@@ -7740,7 +7740,7 @@
         <v>14400</v>
       </c>
       <c r="E309">
-        <v>2455.585256013827</v>
+        <v>2719.321519750091</v>
       </c>
       <c r="F309">
         <v>32</v>
@@ -7760,7 +7760,7 @@
         <v>14400</v>
       </c>
       <c r="E310">
-        <v>2053.570603999175</v>
+        <v>2339.284889713461</v>
       </c>
       <c r="F310">
         <v>32</v>
@@ -7780,7 +7780,7 @@
         <v>14400</v>
       </c>
       <c r="E311">
-        <v>2455.585256013827</v>
+        <v>2719.321519750091</v>
       </c>
       <c r="F311">
         <v>32</v>
@@ -7800,7 +7800,7 @@
         <v>12000</v>
       </c>
       <c r="E312">
-        <v>1886.903937332509</v>
+        <v>2124.999175427747</v>
       </c>
       <c r="F312">
         <v>32</v>
@@ -7820,7 +7820,7 @@
         <v>15200</v>
       </c>
       <c r="E313">
-        <v>1950.396000824572</v>
+        <v>2251.983302411874</v>
       </c>
       <c r="F313">
         <v>33.77777777777778</v>
@@ -7840,7 +7840,7 @@
         <v>12000</v>
       </c>
       <c r="E314">
-        <v>2378.66217909075</v>
+        <v>2598.44239887097</v>
       </c>
       <c r="F314">
         <v>32</v>
@@ -7860,7 +7860,7 @@
         <v>10000</v>
       </c>
       <c r="E315">
-        <v>1787.697588126159</v>
+        <v>1986.110286538858</v>
       </c>
       <c r="F315">
         <v>32.05128205128205</v>
@@ -7880,7 +7880,7 @@
         <v>14400</v>
       </c>
       <c r="E316">
-        <v>1928.570603999175</v>
+        <v>2214.284889713461</v>
       </c>
       <c r="F316">
         <v>32</v>
@@ -7900,7 +7900,7 @@
         <v>28800</v>
       </c>
       <c r="E317">
-        <v>2214.284889713461</v>
+        <v>2785.713461142032</v>
       </c>
       <c r="F317">
         <v>64</v>
@@ -7920,7 +7920,7 @@
         <v>14400</v>
       </c>
       <c r="E318">
-        <v>1928.570603999175</v>
+        <v>2214.284889713461</v>
       </c>
       <c r="F318">
         <v>32</v>
@@ -7940,7 +7940,7 @@
         <v>15000</v>
       </c>
       <c r="E319">
-        <v>2741.037898609327</v>
+        <v>2996.139939425653</v>
       </c>
       <c r="F319">
         <v>33.33333333333334</v>
@@ -7960,7 +7960,7 @@
         <v>28800</v>
       </c>
       <c r="E320">
-        <v>2576.464376892948</v>
+        <v>3103.936904365476</v>
       </c>
       <c r="F320">
         <v>64</v>
@@ -7980,7 +7980,7 @@
         <v>17600</v>
       </c>
       <c r="E321">
-        <v>2948.520891806606</v>
+        <v>3247.840619697762</v>
       </c>
       <c r="F321">
         <v>39.11111111111111</v>
@@ -8000,7 +8000,7 @@
         <v>8400</v>
       </c>
       <c r="E322">
-        <v>1899.999175427747</v>
+        <v>2066.665842094413</v>
       </c>
       <c r="F322">
         <v>32.06106870229008</v>
@@ -8020,7 +8020,7 @@
         <v>12000</v>
       </c>
       <c r="E323">
-        <v>2357.783058211629</v>
+        <v>2577.563277991849</v>
       </c>
       <c r="F323">
         <v>32</v>
@@ -8040,7 +8040,7 @@
         <v>14400</v>
       </c>
       <c r="E324">
-        <v>2339.284889713461</v>
+        <v>2624.999175427747</v>
       </c>
       <c r="F324">
         <v>32</v>
@@ -8060,7 +8060,7 @@
         <v>15200</v>
       </c>
       <c r="E325">
-        <v>2224.205524634096</v>
+        <v>2525.792826221398</v>
       </c>
       <c r="F325">
         <v>33.77777777777778</v>
@@ -8080,7 +8080,7 @@
         <v>12000</v>
       </c>
       <c r="E326">
-        <v>1755.951556380128</v>
+        <v>1994.046794475366</v>
       </c>
       <c r="F326">
         <v>32</v>
@@ -8100,7 +8100,7 @@
         <v>6000</v>
       </c>
       <c r="E327">
-        <v>1906.745207173778</v>
+        <v>2025.792826221397</v>
       </c>
       <c r="F327">
         <v>32.0855614973262</v>
@@ -8120,7 +8120,7 @@
         <v>12000</v>
       </c>
       <c r="E328">
-        <v>2025.792826221397</v>
+        <v>2263.888064316635</v>
       </c>
       <c r="F328">
         <v>32</v>
@@ -8140,7 +8140,7 @@
         <v>14400</v>
       </c>
       <c r="E329">
-        <v>2601.582116296402</v>
+        <v>2846.480075480075</v>
       </c>
       <c r="F329">
         <v>32</v>
@@ -8160,7 +8160,7 @@
         <v>28800</v>
       </c>
       <c r="E330">
-        <v>2846.480075480075</v>
+        <v>3336.275993847422</v>
       </c>
       <c r="F330">
         <v>64</v>
@@ -8180,7 +8180,7 @@
         <v>14400</v>
       </c>
       <c r="E331">
-        <v>2340.475365903937</v>
+        <v>2626.189651618223</v>
       </c>
       <c r="F331">
         <v>32</v>
@@ -8200,7 +8200,7 @@
         <v>28800</v>
       </c>
       <c r="E332">
-        <v>2588.55228898086</v>
+        <v>3116.024816453388</v>
       </c>
       <c r="F332">
         <v>64</v>
@@ -8220,7 +8220,7 @@
         <v>14000</v>
       </c>
       <c r="E333">
-        <v>2656.003885003885</v>
+        <v>2894.099123099123</v>
       </c>
       <c r="F333">
         <v>32.03661327231121</v>
@@ -8240,7 +8240,7 @@
         <v>4800</v>
       </c>
       <c r="E334">
-        <v>2656.003885003885</v>
+        <v>2894.099123099123</v>
       </c>
       <c r="F334">
         <v>32</v>
@@ -8260,7 +8260,7 @@
         <v>5000</v>
       </c>
       <c r="E335">
-        <v>2124.999175427747</v>
+        <v>2224.205524634096</v>
       </c>
       <c r="F335">
         <v>32.05128205128205</v>
@@ -8280,7 +8280,7 @@
         <v>30000</v>
       </c>
       <c r="E336">
-        <v>2455.585256013827</v>
+        <v>3005.035805464377</v>
       </c>
       <c r="F336">
         <v>66.66666666666667</v>
@@ -8300,7 +8300,7 @@
         <v>14000</v>
       </c>
       <c r="E337">
-        <v>2164.681715110286</v>
+        <v>2442.459492888064</v>
       </c>
       <c r="F337">
         <v>32.03661327231121</v>
@@ -8320,7 +8320,7 @@
         <v>19200</v>
       </c>
       <c r="E338">
-        <v>2331.348381776953</v>
+        <v>2712.300762729334</v>
       </c>
       <c r="F338">
         <v>42.66666666666666</v>
@@ -8340,7 +8340,7 @@
         <v>12000</v>
       </c>
       <c r="E339">
-        <v>2124.999175427747</v>
+        <v>2363.094413522985</v>
       </c>
       <c r="F339">
         <v>32</v>
@@ -8360,7 +8360,7 @@
         <v>7200</v>
       </c>
       <c r="E340">
-        <v>1541.665842094414</v>
+        <v>1684.522984951557</v>
       </c>
       <c r="F340">
         <v>32</v>
@@ -8380,7 +8380,7 @@
         <v>17000</v>
       </c>
       <c r="E341">
-        <v>3030.15354486783</v>
+        <v>3319.269191126333</v>
       </c>
       <c r="F341">
         <v>37.77777777777778</v>
@@ -8400,7 +8400,7 @@
         <v>43200</v>
       </c>
       <c r="E342">
-        <v>2649.201163915449</v>
+        <v>3383.89504146647</v>
       </c>
       <c r="F342">
         <v>96</v>
@@ -8420,7 +8420,7 @@
         <v>15000</v>
       </c>
       <c r="E343">
-        <v>2156.745207173778</v>
+        <v>2454.364254792826</v>
       </c>
       <c r="F343">
         <v>33.33333333333334</v>
@@ -8440,7 +8440,7 @@
         <v>28800</v>
       </c>
       <c r="E344">
-        <v>2472.068772497344</v>
+        <v>2999.541299969871</v>
       </c>
       <c r="F344">
         <v>64</v>
@@ -8460,7 +8460,7 @@
         <v>28800</v>
       </c>
       <c r="E345">
-        <v>2815.867830582116</v>
+        <v>3305.663748949462</v>
       </c>
       <c r="F345">
         <v>64</v>
@@ -8480,7 +8480,7 @@
         <v>14400</v>
       </c>
       <c r="E346">
-        <v>2587.453387881959</v>
+        <v>2851.189651618223</v>
       </c>
       <c r="F346">
         <v>32</v>
@@ -8500,7 +8500,7 @@
         <v>17200</v>
       </c>
       <c r="E347">
-        <v>2532.508332936904</v>
+        <v>2847.526647955219</v>
       </c>
       <c r="F347">
         <v>38.22222222222222</v>
@@ -8520,7 +8520,7 @@
         <v>10000</v>
       </c>
       <c r="E348">
-        <v>2224.205524634096</v>
+        <v>2422.618223046794</v>
       </c>
       <c r="F348">
         <v>32.05128205128205</v>
@@ -8540,7 +8540,7 @@
         <v>8000</v>
       </c>
       <c r="E349">
-        <v>2065.475365903937</v>
+        <v>2224.205524634096</v>
       </c>
       <c r="F349">
         <v>32</v>
@@ -8560,7 +8560,7 @@
         <v>36000</v>
       </c>
       <c r="E350">
-        <v>2938.316810173953</v>
+        <v>3550.561708133137</v>
       </c>
       <c r="F350">
         <v>80</v>
@@ -8580,7 +8580,7 @@
         <v>56600</v>
       </c>
       <c r="E351">
-        <v>3181.514089085517</v>
+        <v>4144.099123099122</v>
       </c>
       <c r="F351">
         <v>125.7777777777778</v>
@@ -8600,7 +8600,7 @@
         <v>14400</v>
       </c>
       <c r="E352">
-        <v>2846.480075480075</v>
+        <v>3091.378034663749</v>
       </c>
       <c r="F352">
         <v>32</v>
@@ -8620,7 +8620,7 @@
         <v>28800</v>
       </c>
       <c r="E353">
-        <v>3091.378034663749</v>
+        <v>3581.173953031095</v>
       </c>
       <c r="F353">
         <v>64</v>
@@ -8640,7 +8640,7 @@
         <v>43200</v>
       </c>
       <c r="E354">
-        <v>3581.173953031095</v>
+        <v>4315.867830582115</v>
       </c>
       <c r="F354">
         <v>96</v>
@@ -8660,7 +8660,7 @@
         <v>14400</v>
       </c>
       <c r="E355">
-        <v>2588.55228898086</v>
+        <v>2852.288552717124</v>
       </c>
       <c r="F355">
         <v>32</v>
@@ -8680,7 +8680,7 @@
         <v>28800</v>
       </c>
       <c r="E356">
-        <v>2340.475365903937</v>
+        <v>2911.903937332509</v>
       </c>
       <c r="F356">
         <v>64</v>
@@ -8700,7 +8700,7 @@
         <v>16000</v>
       </c>
       <c r="E357">
-        <v>2928.112728541299</v>
+        <v>3200.221572078714</v>
       </c>
       <c r="F357">
         <v>35.55555555555556</v>
@@ -8720,7 +8720,7 @@
         <v>5500</v>
       </c>
       <c r="E358">
-        <v>2425.548625977197</v>
+        <v>2526.281226709798</v>
       </c>
       <c r="F358">
         <v>32.16374269005848</v>
@@ -8740,7 +8740,7 @@
         <v>28800</v>
       </c>
       <c r="E359">
-        <v>2953.622932622932</v>
+        <v>3443.418850990279</v>
       </c>
       <c r="F359">
         <v>64</v>
@@ -8760,7 +8760,7 @@
         <v>20400</v>
       </c>
       <c r="E360">
-        <v>3285.255585684157</v>
+        <v>3632.194361194361</v>
       </c>
       <c r="F360">
         <v>45.33333333333334</v>
@@ -8780,7 +8780,7 @@
         <v>10000</v>
       </c>
       <c r="E361">
-        <v>2507.96620839478</v>
+        <v>2691.116391544963</v>
       </c>
       <c r="F361">
         <v>32.05128205128205</v>
@@ -8800,7 +8800,7 @@
         <v>14400</v>
       </c>
       <c r="E362">
-        <v>2588.55228898086</v>
+        <v>2852.288552717124</v>
       </c>
       <c r="F362">
         <v>32</v>
@@ -8820,7 +8820,7 @@
         <v>16000</v>
       </c>
       <c r="E363">
-        <v>2455.585256013827</v>
+        <v>2748.62554905412</v>
       </c>
       <c r="F363">
         <v>35.55555555555556</v>
@@ -8840,7 +8840,7 @@
         <v>14000</v>
       </c>
       <c r="E364">
-        <v>2382.325182753754</v>
+        <v>2638.735439164011</v>
       </c>
       <c r="F364">
         <v>32.03661327231121</v>
@@ -8860,7 +8860,7 @@
         <v>19000</v>
       </c>
       <c r="E365">
-        <v>3353.282796568511</v>
+        <v>3676.412048269191</v>
       </c>
       <c r="F365">
         <v>42.22222222222222</v>
@@ -8880,7 +8880,7 @@
         <v>17000</v>
       </c>
       <c r="E366">
-        <v>2466.574267002838</v>
+        <v>2777.929578358149</v>
       </c>
       <c r="F366">
         <v>37.77777777777778</v>
@@ -8900,7 +8900,7 @@
         <v>28800</v>
       </c>
       <c r="E367">
-        <v>3060.76578976579</v>
+        <v>3550.561708133137</v>
       </c>
       <c r="F367">
         <v>64</v>
@@ -8920,7 +8920,7 @@
         <v>25000</v>
       </c>
       <c r="E368">
-        <v>2279.761080189651</v>
+        <v>2775.792826221397</v>
       </c>
       <c r="F368">
         <v>55.55555555555556</v>
@@ -8940,7 +8940,7 @@
         <v>43200</v>
       </c>
       <c r="E369">
-        <v>3550.561708133136</v>
+        <v>4285.255585684156</v>
       </c>
       <c r="F369">
         <v>96</v>
@@ -8960,7 +8960,7 @@
         <v>28800</v>
       </c>
       <c r="E370">
-        <v>3060.76578976579</v>
+        <v>3550.561708133137</v>
       </c>
       <c r="F370">
         <v>64</v>
@@ -8980,7 +8980,7 @@
         <v>12000</v>
       </c>
       <c r="E371">
-        <v>2437.270237698809</v>
+        <v>2657.050457479029</v>
       </c>
       <c r="F371">
         <v>32</v>
@@ -9000,7 +9000,7 @@
         <v>10000</v>
       </c>
       <c r="E372">
-        <v>2263.888064316635</v>
+        <v>2462.300762729334</v>
       </c>
       <c r="F372">
         <v>32.05128205128205</v>
@@ -9020,7 +9020,7 @@
         <v>28800</v>
       </c>
       <c r="E373">
-        <v>2220.237270665842</v>
+        <v>2791.665842094413</v>
       </c>
       <c r="F373">
         <v>64</v>
@@ -9040,7 +9040,7 @@
         <v>28800</v>
       </c>
       <c r="E374">
-        <v>3336.275993847422</v>
+        <v>3826.071912214768</v>
       </c>
       <c r="F374">
         <v>64</v>
@@ -9060,7 +9060,7 @@
         <v>43200</v>
       </c>
       <c r="E375">
-        <v>3826.071912214769</v>
+        <v>4560.765789765789</v>
       </c>
       <c r="F375">
         <v>96</v>
@@ -9080,7 +9080,7 @@
         <v>43200</v>
       </c>
       <c r="E376">
-        <v>3061.786197929055</v>
+        <v>3796.480075480075</v>
       </c>
       <c r="F376">
         <v>96</v>
@@ -9100,7 +9100,7 @@
         <v>28800</v>
       </c>
       <c r="E377">
-        <v>3061.786197929055</v>
+        <v>3551.582116296401</v>
       </c>
       <c r="F377">
         <v>64</v>
@@ -9120,7 +9120,7 @@
         <v>18000</v>
       </c>
       <c r="E378">
-        <v>3234.235177520891</v>
+        <v>3540.357626500483</v>
       </c>
       <c r="F378">
         <v>40</v>
@@ -9140,7 +9140,7 @@
         <v>14400</v>
       </c>
       <c r="E379">
-        <v>3305.663748949463</v>
+        <v>3550.561708133136</v>
       </c>
       <c r="F379">
         <v>32</v>
@@ -9160,7 +9160,7 @@
         <v>28800</v>
       </c>
       <c r="E380">
-        <v>3443.418850990279</v>
+        <v>3933.214769357626</v>
       </c>
       <c r="F380">
         <v>64</v>
@@ -9180,7 +9180,7 @@
         <v>28800</v>
       </c>
       <c r="E381">
-        <v>2713.827014255585</v>
+        <v>3203.622932622932</v>
       </c>
       <c r="F381">
         <v>64</v>
@@ -9200,7 +9200,7 @@
         <v>18000</v>
       </c>
       <c r="E382">
-        <v>2754.643340786198</v>
+        <v>3060.76578976579</v>
       </c>
       <c r="F382">
         <v>40</v>
@@ -9220,7 +9220,7 @@
         <v>16000</v>
       </c>
       <c r="E383">
-        <v>2652.602524459667</v>
+        <v>2924.711367997082</v>
       </c>
       <c r="F383">
         <v>35.55555555555556</v>
@@ -9240,7 +9240,7 @@
         <v>21000</v>
       </c>
       <c r="E384">
-        <v>3710.425653711367</v>
+        <v>4067.568510854224</v>
       </c>
       <c r="F384">
         <v>46.66666666666666</v>
@@ -9260,7 +9260,7 @@
         <v>50000</v>
       </c>
       <c r="E385">
-        <v>3309.065109493681</v>
+        <v>4159.405245548102</v>
       </c>
       <c r="F385">
         <v>111.1111111111111</v>
@@ -9280,7 +9280,7 @@
         <v>43200</v>
       </c>
       <c r="E386">
-        <v>3795.45966731681</v>
+        <v>4530.15354486783</v>
       </c>
       <c r="F386">
         <v>96</v>
@@ -9300,7 +9300,7 @@
         <v>14000</v>
       </c>
       <c r="E387">
-        <v>2669.609327180755</v>
+        <v>2907.704565275993</v>
       </c>
       <c r="F387">
         <v>32.03661327231121</v>
@@ -9320,7 +9320,7 @@
         <v>12000</v>
       </c>
       <c r="E388">
-        <v>2473.900274328846</v>
+        <v>2693.680494109065</v>
       </c>
       <c r="F388">
         <v>32</v>
@@ -9340,7 +9340,7 @@
         <v>28800</v>
       </c>
       <c r="E389">
-        <v>2339.284889713461</v>
+        <v>2910.713461142032</v>
       </c>
       <c r="F389">
         <v>64</v>
@@ -9360,7 +9360,7 @@
         <v>43200</v>
       </c>
       <c r="E390">
-        <v>3796.480075480075</v>
+        <v>4531.173953031095</v>
       </c>
       <c r="F390">
         <v>96</v>
@@ -9380,7 +9380,7 @@
         <v>43200</v>
       </c>
       <c r="E391">
-        <v>3061.786197929055</v>
+        <v>3796.480075480075</v>
       </c>
       <c r="F391">
         <v>96</v>
@@ -9400,7 +9400,7 @@
         <v>50000</v>
       </c>
       <c r="E392">
-        <v>3604.983476840619</v>
+        <v>4455.32361289504</v>
       </c>
       <c r="F392">
         <v>111.1111111111111</v>
@@ -9420,7 +9420,7 @@
         <v>10000</v>
       </c>
       <c r="E393">
-        <v>3231.854225139939</v>
+        <v>3401.922252350823</v>
       </c>
       <c r="F393">
         <v>32.05128205128205</v>
@@ -9440,7 +9440,7 @@
         <v>28800</v>
       </c>
       <c r="E394">
-        <v>2815.867830582116</v>
+        <v>3305.663748949462</v>
       </c>
       <c r="F394">
         <v>64</v>
@@ -9460,7 +9460,7 @@
         <v>50000</v>
       </c>
       <c r="E395">
-        <v>2962.126333983476</v>
+        <v>3812.466470037898</v>
       </c>
       <c r="F395">
         <v>111.1111111111111</v>
@@ -9480,7 +9480,7 @@
         <v>14400</v>
       </c>
       <c r="E396">
-        <v>3306.684157112728</v>
+        <v>3551.582116296401</v>
       </c>
       <c r="F396">
         <v>32</v>
@@ -9500,7 +9500,7 @@
         <v>30000</v>
       </c>
       <c r="E397">
-        <v>2455.585256013827</v>
+        <v>3005.035805464377</v>
       </c>
       <c r="F397">
         <v>66.66666666666667</v>
@@ -9520,7 +9520,7 @@
         <v>22000</v>
       </c>
       <c r="E398">
-        <v>3128.793000650143</v>
+        <v>3502.942660514089</v>
       </c>
       <c r="F398">
         <v>48.88888888888889</v>
@@ -9540,7 +9540,7 @@
         <v>55000</v>
       </c>
       <c r="E399">
-        <v>3394.099123099123</v>
+        <v>4329.473272758986</v>
       </c>
       <c r="F399">
         <v>122.2222222222222</v>
@@ -9560,7 +9560,7 @@
         <v>24000</v>
       </c>
       <c r="E400">
-        <v>3536.956265956265</v>
+        <v>3945.119531262388</v>
       </c>
       <c r="F400">
         <v>53.33333333333334</v>

</xml_diff>